<commit_message>
add and link open document tools and correct typo in tools
</commit_message>
<xml_diff>
--- a/docs/00_Tools/05_05_DE_Life-Cycle-Tool.xlsx
+++ b/docs/00_Tools/05_05_DE_Life-Cycle-Tool.xlsx
@@ -437,13 +437,13 @@
     </r>
   </si>
   <si>
-    <t>Übersetzung: Katharina Zinke, Unversitätsbibliothek Tübingen</t>
-  </si>
-  <si>
     <t>Lizenziert unter CC BY 4.0</t>
   </si>
   <si>
     <t xml:space="preserve">Original: www.learningspacetoolkit.org </t>
+  </si>
+  <si>
+    <t>Übersetzung: Katharina Zinke, Universitätsbibliothek Tübingen</t>
   </si>
 </sst>
 </file>
@@ -1260,6 +1260,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1392,7 +1393,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1532,28 +1532,6 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.24681581225747357"/>
-                      <c:h val="5.7005193083399817E-2"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000016-2E97-4E1C-B4A6-CEE86B66F39C}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -3370,7 +3348,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3405,20 +3383,20 @@
     <row r="2" spans="1:15" ht="66.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
       <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:15" ht="6.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -3444,38 +3422,38 @@
       <c r="C4" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
       <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
       <c r="O5" s="26"/>
     </row>
     <row r="6" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3501,19 +3479,19 @@
       <c r="C7" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
       <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3536,7 +3514,7 @@
     <row r="9" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="100" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="79" t="s">
@@ -3557,7 +3535,7 @@
     <row r="10" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="100"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
@@ -3574,26 +3552,26 @@
     <row r="11" spans="1:15" s="31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="107" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="108"/>
-      <c r="L11" s="108"/>
-      <c r="M11" s="108"/>
-      <c r="N11" s="108"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
       <c r="O11" s="30"/>
     </row>
     <row r="12" spans="1:15" s="31" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="100"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
@@ -3610,26 +3588,26 @@
     <row r="13" spans="1:15" s="31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="94" t="s">
+      <c r="C13" s="101"/>
+      <c r="D13" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="95"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="95"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
       <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" s="31" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="100"/>
+      <c r="C14" s="101"/>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
@@ -3646,20 +3624,20 @@
     <row r="15" spans="1:15" s="40" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="96" t="s">
+      <c r="C15" s="101"/>
+      <c r="D15" s="97" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="99"/>
       <c r="O15" s="21"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3683,8 +3661,8 @@
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="138" t="s">
-        <v>88</v>
+      <c r="D17" s="94" t="s">
+        <v>87</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -3702,8 +3680,8 @@
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
-      <c r="D18" s="138" t="s">
-        <v>86</v>
+      <c r="D18" s="94" t="s">
+        <v>88</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
@@ -3721,8 +3699,8 @@
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
-      <c r="D19" s="138" t="s">
-        <v>87</v>
+      <c r="D19" s="94" t="s">
+        <v>86</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
@@ -3795,19 +3773,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:222" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
     </row>
     <row r="2" spans="1:222" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="69" t="s">
@@ -3816,14 +3794,14 @@
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
     </row>
     <row r="3" spans="1:222" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -3839,19 +3817,19 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:222" s="19" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
       <c r="L4" s="18"/>
       <c r="M4" s="43"/>
       <c r="N4" s="43"/>
@@ -4289,36 +4267,36 @@
       <c r="HN5" s="43"/>
     </row>
     <row r="6" spans="1:222" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
     </row>
     <row r="7" spans="1:222" s="3" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="130"/>
       <c r="G7" s="32"/>
-      <c r="H7" s="130" t="s">
+      <c r="H7" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="131"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="133"/>
       <c r="L7" s="14"/>
       <c r="M7" s="44"/>
       <c r="N7" s="44"/>
@@ -8941,14 +8919,14 @@
       <c r="HN26" s="42"/>
     </row>
     <row r="27" spans="1:222" s="6" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="115"/>
-      <c r="B27" s="109" t="s">
+      <c r="A27" s="116"/>
+      <c r="B27" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="112"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -9166,7 +9144,7 @@
       <c r="HN27" s="42"/>
     </row>
     <row r="28" spans="1:222" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116"/>
+      <c r="A28" s="117"/>
       <c r="B28" s="59" t="s">
         <v>26</v>
       </c>
@@ -9393,7 +9371,7 @@
       <c r="HN28" s="44"/>
     </row>
     <row r="29" spans="1:222" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="117"/>
+      <c r="A29" s="118"/>
       <c r="B29" s="61">
         <v>1</v>
       </c>
@@ -10788,16 +10766,16 @@
       <c r="HN34" s="42"/>
     </row>
     <row r="35" spans="1:222" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="118" t="s">
+      <c r="A35" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="112" t="s">
+      <c r="B35" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="114"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="114"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="115"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -11015,7 +10993,7 @@
       <c r="HN35" s="42"/>
     </row>
     <row r="36" spans="1:222" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="119"/>
+      <c r="A36" s="120"/>
       <c r="B36" s="56" t="s">
         <v>48</v>
       </c>
@@ -11242,7 +11220,7 @@
       <c r="HN36" s="44"/>
     </row>
     <row r="37" spans="1:222" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="120"/>
+      <c r="A37" s="121"/>
       <c r="B37" s="58">
         <v>1</v>
       </c>
@@ -14709,9 +14687,9 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -14724,11 +14702,11 @@
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -14741,11 +14719,11 @@
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -14766,35 +14744,35 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="137"/>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" s="43" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="124" t="s">
+      <c r="F5" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>

</xml_diff>